<commit_message>
Apply LCFS to shipping in policy case
</commit_message>
<xml_diff>
--- a/InputData/trans/PVTStL/Policy Veh Types Subject to LCFS.xlsx
+++ b/InputData/trans/PVTStL/Policy Veh Types Subject to LCFS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\trans\PVTStL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\trans\PVTStL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE39D9D-8C5C-4506-8739-69D1A3827F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8B7640-3F18-4F5C-A9FF-A8B089B6F820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="720" windowWidth="26730" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -523,7 +523,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,10 +593,10 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>